<commit_message>
se mejoran graficas excel y se agrega guía, el informe ya está entregado
</commit_message>
<xml_diff>
--- a/DatosLab3.xlsx
+++ b/DatosLab3.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\UMNG\2022-1\Control\Lab Control\CTRL-Lab3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\UMNG\2022-1\local work\CTRL-Lab3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9F7EBC7-9B7B-4AE2-AEC2-E60D41A8944C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0138328E-6755-4111-9FAD-62DEBC73AC66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -79,7 +79,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -87,12 +87,28 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -175,7 +191,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-CO"/>
+          <a:endParaRPr lang="es-MX"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -256,8 +272,8 @@
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-0.43410389326334209"/>
-                  <c:y val="-2.8194444444444466E-2"/>
+                  <c:x val="-0.38023880014511546"/>
+                  <c:y val="4.2238258571822762E-3"/>
                 </c:manualLayout>
               </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
@@ -285,7 +301,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="es-CO"/>
+                  <a:endParaRPr lang="es-MX"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -478,7 +494,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-CO"/>
+            <a:endParaRPr lang="es-MX"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="580680656"/>
@@ -540,7 +556,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-CO"/>
+            <a:endParaRPr lang="es-MX"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="580681640"/>
@@ -581,7 +597,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="es-CO"/>
+      <a:endParaRPr lang="es-MX"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -662,7 +678,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-CO"/>
+          <a:endParaRPr lang="es-MX"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -758,7 +774,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="es-CO"/>
+                  <a:endParaRPr lang="es-MX"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -951,7 +967,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-CO"/>
+            <a:endParaRPr lang="es-MX"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="582653880"/>
@@ -1013,7 +1029,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-CO"/>
+            <a:endParaRPr lang="es-MX"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="582653552"/>
@@ -1054,7 +1070,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="es-CO"/>
+      <a:endParaRPr lang="es-MX"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1130,7 +1146,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-CO"/>
+          <a:endParaRPr lang="es-MX"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -1282,7 +1298,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="es-CO"/>
+                  <a:endParaRPr lang="es-MX"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -1576,7 +1592,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-CO"/>
+            <a:endParaRPr lang="es-MX"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="590629744"/>
@@ -1639,7 +1655,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-CO"/>
+            <a:endParaRPr lang="es-MX"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="590628432"/>
@@ -1687,7 +1703,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="es-CO"/>
+      <a:endParaRPr lang="es-MX"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1769,7 +1785,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-CO"/>
+          <a:endParaRPr lang="es-MX"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -1879,7 +1895,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="es-CO"/>
+                  <a:endParaRPr lang="es-MX"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -2072,7 +2088,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-CO"/>
+            <a:endParaRPr lang="es-MX"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="582671936"/>
@@ -2134,7 +2150,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-CO"/>
+            <a:endParaRPr lang="es-MX"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="582671280"/>
@@ -2175,7 +2191,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="es-CO"/>
+      <a:endParaRPr lang="es-MX"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -4858,31 +4874,31 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="G1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
         <v>5.5</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="1">
         <v>619</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="1">
         <v>1.67</v>
       </c>
       <c r="E2" t="s">
@@ -4895,15 +4911,15 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
         <f>A2+0.2</f>
         <v>5.7</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="1">
         <v>666</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="1">
         <v>1.82</v>
       </c>
       <c r="E3" t="s">
@@ -4917,15 +4933,15 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A4">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
         <f t="shared" ref="A4:A17" si="0">A3+0.2</f>
         <v>5.9</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="1">
         <v>713</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="1">
         <v>1.88</v>
       </c>
       <c r="E4" t="s">
@@ -4935,159 +4951,159 @@
         <v>2.25</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A5">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
         <f t="shared" si="0"/>
         <v>6.1000000000000005</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="1">
         <v>756</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="1">
         <v>1.64</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A6">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
         <f t="shared" si="0"/>
         <v>6.3000000000000007</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="1">
         <v>786</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="1">
         <v>1.9</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
         <f t="shared" si="0"/>
         <v>6.5000000000000009</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="1">
         <v>835</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A8">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
         <f t="shared" si="0"/>
         <v>6.7000000000000011</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="1">
         <v>875</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="1">
         <v>2.13</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A9">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
         <f t="shared" si="0"/>
         <v>6.9000000000000012</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="1">
         <v>930</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="1">
         <v>2.37</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A10">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
         <f t="shared" si="0"/>
         <v>7.1000000000000014</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="1">
         <v>978</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="1">
         <v>2.5299999999999998</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A11">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
         <f t="shared" si="0"/>
         <v>7.3000000000000016</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="1">
         <v>1028</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="1">
         <v>2.79</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A12">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
         <f t="shared" si="0"/>
         <v>7.5000000000000018</v>
       </c>
-      <c r="B12">
+      <c r="B12" s="1">
         <v>1068</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="1">
         <v>2.7</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A13">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
         <f t="shared" si="0"/>
         <v>7.700000000000002</v>
       </c>
-      <c r="B13">
+      <c r="B13" s="1">
         <v>1120</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="1">
         <v>2.8</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A14">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
         <f>A13+0.2</f>
         <v>7.9000000000000021</v>
       </c>
-      <c r="B14">
+      <c r="B14" s="1">
         <v>1160</v>
       </c>
-      <c r="C14">
+      <c r="C14" s="1">
         <v>2.82</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A15">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
         <f t="shared" si="0"/>
         <v>8.1000000000000014</v>
       </c>
-      <c r="B15">
+      <c r="B15" s="1">
         <v>1200</v>
       </c>
-      <c r="C15">
+      <c r="C15" s="1">
         <v>2.96</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A16">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
         <f t="shared" si="0"/>
         <v>8.3000000000000007</v>
       </c>
-      <c r="B16">
+      <c r="B16" s="1">
         <v>1242</v>
       </c>
-      <c r="C16">
+      <c r="C16" s="1">
         <v>3.09</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A17">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
         <f t="shared" si="0"/>
         <v>8.5</v>
       </c>
-      <c r="B17">
+      <c r="B17" s="1">
         <v>1282</v>
       </c>
-      <c r="C17">
+      <c r="C17" s="1">
         <v>3.1</v>
       </c>
       <c r="F17">
@@ -5097,6 +5113,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>